<commit_message>
added some testing for power, current adc works fine now conversion is still not good.
</commit_message>
<xml_diff>
--- a/Basic/Tony_Huang/Book1.xlsx
+++ b/Basic/Tony_Huang/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qhua835\Downloads\ec209-project-2023_team-22\Basic\Tony_Huang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Sem 2\COMPSYS209\ec209-project-2023_team-22\Basic\Tony_Huang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF6097-439D-468F-88F8-4A8D0725DB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CCF63D-134D-482D-8CA5-B4B264AEF3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7E05461-0193-4B7E-975C-B664CF06D085}"/>
   </bookViews>
@@ -4021,8 +4021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F34B049-2C4F-43C1-AAC7-5FF518FB1B35}">
   <dimension ref="A1:CD298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I116" sqref="I116"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R212" sqref="R212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>